<commit_message>
fix expiryDate typo in 160301 concept
</commit_message>
<xml_diff>
--- a/VocabolariControllati/classifications-for-transparency/transparency-obligation/transparency-obligation.xlsx
+++ b/VocabolariControllati/classifications-for-transparency/transparency-obligation/transparency-obligation.xlsx
@@ -2687,7 +2687,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="61.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="40.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="122.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="29.85"/>
   </cols>
   <sheetData>
@@ -23725,7 +23725,7 @@
       <c r="L550" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M550" s="0" t="s">
+      <c r="N550" s="0" t="s">
         <v>669</v>
       </c>
     </row>
@@ -23763,7 +23763,7 @@
       <c r="L551" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M551" s="0" t="s">
+      <c r="N551" s="0" t="s">
         <v>669</v>
       </c>
     </row>
@@ -23801,7 +23801,7 @@
       <c r="L552" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M552" s="0" t="s">
+      <c r="N552" s="0" t="s">
         <v>669</v>
       </c>
     </row>
@@ -23839,7 +23839,7 @@
       <c r="L553" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M553" s="0" t="s">
+      <c r="N553" s="0" t="s">
         <v>669</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix titulus of concept 040102
</commit_message>
<xml_diff>
--- a/VocabolariControllati/classifications-for-transparency/transparency-obligation/transparency-obligation.xlsx
+++ b/VocabolariControllati/classifications-for-transparency/transparency-obligation/transparency-obligation.xlsx
@@ -619,6 +619,9 @@
     <t xml:space="preserve">040102</t>
   </si>
   <si>
+    <t xml:space="preserve">0402</t>
+  </si>
+  <si>
     <t xml:space="preserve">Obbligo di pubblicazione concernente I titolari di incarichi dirigenziali</t>
   </si>
   <si>
@@ -626,9 +629,6 @@
   </si>
   <si>
     <t xml:space="preserve">040202</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0402</t>
   </si>
   <si>
     <t xml:space="preserve">Obbligo di pubblicazione del numero di posti di funzione disponibili</t>
@@ -13238,16 +13238,16 @@
         <v>81</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D271" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E271" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F271" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G271" s="1" t="s">
         <v>91</v>
@@ -13279,16 +13279,16 @@
         <v>88</v>
       </c>
       <c r="C272" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D272" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E272" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F272" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G272" s="1" t="s">
         <v>91</v>
@@ -13320,16 +13320,16 @@
         <v>90</v>
       </c>
       <c r="C273" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D273" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E273" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F273" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G273" s="1" t="s">
         <v>91</v>
@@ -13361,16 +13361,16 @@
         <v>196</v>
       </c>
       <c r="C274" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D274" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E274" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F274" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G274" s="1" t="s">
         <v>91</v>
@@ -13402,16 +13402,16 @@
         <v>197</v>
       </c>
       <c r="C275" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D275" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E275" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F275" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G275" s="1" t="s">
         <v>91</v>
@@ -13443,16 +13443,16 @@
         <v>81</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D276" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E276" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F276" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G276" s="1" t="s">
         <v>91</v>
@@ -13484,16 +13484,16 @@
         <v>88</v>
       </c>
       <c r="C277" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D277" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E277" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F277" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G277" s="1" t="s">
         <v>91</v>
@@ -13525,16 +13525,16 @@
         <v>90</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D278" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E278" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F278" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G278" s="1" t="s">
         <v>91</v>
@@ -13566,16 +13566,16 @@
         <v>196</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D279" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E279" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F279" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G279" s="1" t="s">
         <v>91</v>
@@ -13607,16 +13607,16 @@
         <v>197</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D280" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E280" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F280" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G280" s="1" t="s">
         <v>91</v>
@@ -13648,16 +13648,16 @@
         <v>81</v>
       </c>
       <c r="C281" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D281" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E281" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F281" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G281" s="1" t="s">
         <v>91</v>
@@ -13689,16 +13689,16 @@
         <v>88</v>
       </c>
       <c r="C282" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D282" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E282" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F282" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G282" s="1" t="s">
         <v>91</v>
@@ -13730,16 +13730,16 @@
         <v>90</v>
       </c>
       <c r="C283" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D283" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E283" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F283" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G283" s="1" t="s">
         <v>91</v>
@@ -13771,16 +13771,16 @@
         <v>196</v>
       </c>
       <c r="C284" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D284" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E284" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F284" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G284" s="1" t="s">
         <v>91</v>
@@ -13812,16 +13812,16 @@
         <v>197</v>
       </c>
       <c r="C285" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D285" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E285" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F285" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G285" s="1" t="s">
         <v>91</v>
@@ -13853,16 +13853,16 @@
         <v>81</v>
       </c>
       <c r="C286" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D286" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E286" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F286" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G286" s="1" t="s">
         <v>84</v>
@@ -13894,16 +13894,16 @@
         <v>88</v>
       </c>
       <c r="C287" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D287" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E287" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F287" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G287" s="1" t="s">
         <v>84</v>
@@ -13935,16 +13935,16 @@
         <v>90</v>
       </c>
       <c r="C288" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D288" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E288" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F288" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G288" s="1" t="s">
         <v>84</v>
@@ -13976,16 +13976,16 @@
         <v>196</v>
       </c>
       <c r="C289" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D289" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E289" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F289" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G289" s="1" t="s">
         <v>84</v>
@@ -14017,16 +14017,16 @@
         <v>197</v>
       </c>
       <c r="C290" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D290" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E290" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F290" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G290" s="1" t="s">
         <v>84</v>
@@ -14058,16 +14058,16 @@
         <v>81</v>
       </c>
       <c r="C291" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D291" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E291" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F291" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G291" s="1" t="s">
         <v>84</v>
@@ -14099,16 +14099,16 @@
         <v>88</v>
       </c>
       <c r="C292" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D292" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E292" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F292" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G292" s="1" t="s">
         <v>84</v>
@@ -14140,16 +14140,16 @@
         <v>90</v>
       </c>
       <c r="C293" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D293" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E293" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F293" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G293" s="1" t="s">
         <v>84</v>
@@ -14181,16 +14181,16 @@
         <v>196</v>
       </c>
       <c r="C294" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D294" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E294" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F294" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G294" s="1" t="s">
         <v>84</v>
@@ -14222,16 +14222,16 @@
         <v>197</v>
       </c>
       <c r="C295" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D295" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E295" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F295" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G295" s="1" t="s">
         <v>84</v>
@@ -14263,16 +14263,16 @@
         <v>81</v>
       </c>
       <c r="C296" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D296" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E296" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F296" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G296" s="1" t="s">
         <v>84</v>
@@ -14304,16 +14304,16 @@
         <v>88</v>
       </c>
       <c r="C297" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D297" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E297" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F297" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G297" s="1" t="s">
         <v>84</v>
@@ -14345,16 +14345,16 @@
         <v>90</v>
       </c>
       <c r="C298" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D298" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E298" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F298" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G298" s="1" t="s">
         <v>84</v>
@@ -14386,16 +14386,16 @@
         <v>196</v>
       </c>
       <c r="C299" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D299" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E299" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F299" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G299" s="1" t="s">
         <v>84</v>
@@ -14427,16 +14427,16 @@
         <v>197</v>
       </c>
       <c r="C300" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D300" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E300" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F300" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G300" s="1" t="s">
         <v>84</v>
@@ -14468,16 +14468,16 @@
         <v>81</v>
       </c>
       <c r="C301" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D301" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E301" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F301" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G301" s="1" t="s">
         <v>101</v>
@@ -14509,16 +14509,16 @@
         <v>88</v>
       </c>
       <c r="C302" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D302" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E302" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F302" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G302" s="1" t="s">
         <v>101</v>
@@ -14550,16 +14550,16 @@
         <v>90</v>
       </c>
       <c r="C303" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D303" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E303" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F303" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G303" s="1" t="s">
         <v>101</v>
@@ -14591,16 +14591,16 @@
         <v>196</v>
       </c>
       <c r="C304" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D304" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E304" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F304" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G304" s="1" t="s">
         <v>101</v>
@@ -14632,16 +14632,16 @@
         <v>197</v>
       </c>
       <c r="C305" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D305" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E305" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F305" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G305" s="1" t="s">
         <v>101</v>
@@ -14673,16 +14673,16 @@
         <v>81</v>
       </c>
       <c r="C306" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D306" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E306" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F306" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G306" s="1" t="s">
         <v>101</v>
@@ -14714,16 +14714,16 @@
         <v>88</v>
       </c>
       <c r="C307" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D307" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E307" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F307" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G307" s="1" t="s">
         <v>101</v>
@@ -14755,16 +14755,16 @@
         <v>90</v>
       </c>
       <c r="C308" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D308" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E308" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F308" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G308" s="1" t="s">
         <v>101</v>
@@ -14796,16 +14796,16 @@
         <v>196</v>
       </c>
       <c r="C309" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D309" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E309" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F309" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G309" s="1" t="s">
         <v>101</v>
@@ -14837,16 +14837,16 @@
         <v>197</v>
       </c>
       <c r="C310" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D310" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E310" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F310" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G310" s="1" t="s">
         <v>101</v>
@@ -14878,16 +14878,16 @@
         <v>81</v>
       </c>
       <c r="C311" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D311" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E311" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F311" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G311" s="1" t="s">
         <v>101</v>
@@ -14919,16 +14919,16 @@
         <v>88</v>
       </c>
       <c r="C312" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D312" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E312" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F312" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G312" s="1" t="s">
         <v>101</v>
@@ -14960,16 +14960,16 @@
         <v>90</v>
       </c>
       <c r="C313" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D313" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E313" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F313" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G313" s="1" t="s">
         <v>101</v>
@@ -15001,16 +15001,16 @@
         <v>196</v>
       </c>
       <c r="C314" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D314" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E314" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F314" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G314" s="1" t="s">
         <v>101</v>
@@ -15042,16 +15042,16 @@
         <v>197</v>
       </c>
       <c r="C315" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D315" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E315" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F315" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G315" s="1" t="s">
         <v>101</v>
@@ -15077,10 +15077,10 @@
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C316" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D316" s="1" t="s">
         <v>16</v>
@@ -15112,10 +15112,10 @@
     </row>
     <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C317" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D317" s="1" t="s">
         <v>16</v>
@@ -15147,10 +15147,10 @@
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C318" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D318" s="1" t="s">
         <v>16</v>
@@ -15185,7 +15185,7 @@
         <v>210</v>
       </c>
       <c r="C319" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D319" s="1" t="s">
         <v>16</v>
@@ -15220,7 +15220,7 @@
         <v>210</v>
       </c>
       <c r="C320" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D320" s="1" t="s">
         <v>16</v>
@@ -15255,7 +15255,7 @@
         <v>210</v>
       </c>
       <c r="C321" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D321" s="1" t="s">
         <v>16</v>

</xml_diff>